<commit_message>
survey.json in a hidden sheet
</commit_message>
<xml_diff>
--- a/src/pynanomapper/resource/nmparser/template_pchem.xlsx
+++ b/src/pynanomapper/resource/nmparser/template_pchem.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>General Information</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Study</t>
+  </si>
+  <si>
+    <t>Template name</t>
+  </si>
+  <si>
+    <t>Template acknowledgment</t>
   </si>
 </sst>
 </file>
@@ -183,9 +189,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -533,75 +538,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J17"/>
+  <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -622,43 +643,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="10.5546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
+    <col min="3" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>